<commit_message>
Week Before Final PC Dump
</commit_message>
<xml_diff>
--- a/Drivers/cardinfo.xlsx
+++ b/Drivers/cardinfo.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="495" windowWidth="19875" windowHeight="7650"/>
+    <workbookView xWindow="480" yWindow="555" windowWidth="19875" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="cardinfo" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="49">
   <si>
     <t>0xA2</t>
   </si>
@@ -85,9 +86,6 @@
     <t xml:space="preserve"> 0x04</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0x80</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0x01</t>
   </si>
   <si>
@@ -158,6 +156,12 @@
   </si>
   <si>
     <t>UP Pay Pin</t>
+  </si>
+  <si>
+    <t>Gives App precense and read write information for application</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x88</t>
   </si>
 </sst>
 </file>
@@ -908,7 +912,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -973,6 +977,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1318,7 +1323,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,7 +1352,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="7">
         <v>0</v>
@@ -1380,22 +1385,22 @@
         <v>9</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -1451,13 +1456,13 @@
         <v>14</v>
       </c>
       <c r="R2" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S2" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1501,10 +1506,10 @@
         <v>4</v>
       </c>
       <c r="N3" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>24</v>
       </c>
       <c r="P3" s="14" t="s">
         <v>4</v>
@@ -1514,7 +1519,10 @@
       </c>
       <c r="R3" s="30"/>
       <c r="S3" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="T3" s="52" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1522,7 +1530,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>4</v>
@@ -1546,7 +1554,7 @@
         <v>4</v>
       </c>
       <c r="J4" s="45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="45" t="s">
         <v>4</v>
@@ -1570,10 +1578,10 @@
         <v>4</v>
       </c>
       <c r="R4" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1581,7 +1589,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>4</v>
@@ -1605,7 +1613,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="34" t="s">
         <v>4</v>
@@ -1629,19 +1637,19 @@
         <v>4</v>
       </c>
       <c r="R5" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S5" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="42" t="s">
+      <c r="U5" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="U5" s="38" t="s">
+      <c r="V5" s="47" t="s">
         <v>43</v>
-      </c>
-      <c r="V5" s="47" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1649,7 +1657,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>4</v>
@@ -1673,7 +1681,7 @@
         <v>4</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>4</v>
@@ -1697,7 +1705,7 @@
         <v>4</v>
       </c>
       <c r="R6" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1705,7 +1713,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>4</v>
@@ -1729,7 +1737,7 @@
         <v>4</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>4</v>
@@ -1753,7 +1761,7 @@
         <v>4</v>
       </c>
       <c r="R7" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1761,7 +1769,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>4</v>
@@ -1785,7 +1793,7 @@
         <v>4</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>4</v>
@@ -1808,14 +1816,16 @@
       <c r="Q8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="R8" s="3"/>
+      <c r="R8" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>4</v>
@@ -1839,7 +1849,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>4</v>
@@ -1869,7 +1879,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>4</v>
@@ -1893,7 +1903,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>4</v>
@@ -1916,14 +1926,16 @@
       <c r="Q10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="R10" s="3"/>
+      <c r="R10" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>4</v>
@@ -1947,7 +1959,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>4</v>
@@ -1974,10 +1986,10 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>4</v>
@@ -2001,7 +2013,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>4</v>
@@ -2024,14 +2036,16 @@
       <c r="Q12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R12" s="3"/>
+      <c r="R12" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>4</v>
@@ -2055,7 +2069,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>4</v>
@@ -2082,10 +2096,10 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>4</v>
@@ -2109,7 +2123,7 @@
         <v>4</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K14" s="11" t="s">
         <v>4</v>
@@ -2132,14 +2146,16 @@
       <c r="Q14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R14" s="3"/>
+      <c r="R14" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>4</v>
@@ -2163,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="18" t="s">
         <v>4</v>
@@ -2190,10 +2206,10 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="50" t="s">
         <v>4</v>
@@ -2217,7 +2233,7 @@
         <v>4</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>4</v>
@@ -2241,18 +2257,18 @@
         <v>4</v>
       </c>
       <c r="R16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>4</v>
@@ -2276,7 +2292,7 @@
         <v>4</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" s="18" t="s">
         <v>4</v>

</xml_diff>